<commit_message>
use BLS data for employment
</commit_message>
<xml_diff>
--- a/01_data/occ_occsoc_crosswalk_2000_onward.xlsx
+++ b/01_data/occ_occsoc_crosswalk_2000_onward.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucaskitzmueller/Documents/04_Master/10_Courses/29_Data Visualization/final-project-impact-of-automation-on-labor-markets/01_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F095FBDA-883A-D345-AE9C-E976B0A373E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D704D88B-4D9B-6A47-92C6-B87B450C4317}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="37480" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30790,7 +30790,7 @@
   <dimension ref="A1:C845"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="B348" sqref="B348"/>
+      <selection activeCell="G349" sqref="G349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>